<commit_message>
Added fake news mechanism
</commit_message>
<xml_diff>
--- a/Card_Data.xlsx
+++ b/Card_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samya\Documents\Programming\Github_Repos\Y3Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3604F4-524F-48F9-9617-CF20DB3357C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DFC2E88-CA7D-4C57-8587-8826BFFB5F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{19CA79AA-259F-45F1-9CD4-466022CA0906}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="9">
   <si>
     <t>ID</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>is_checked</t>
   </si>
 </sst>
 </file>
@@ -400,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DA40240-B6B9-4147-8877-CA9E78CDE18C}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,7 +417,7 @@
     <col min="5" max="5" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,8 +436,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -453,8 +459,11 @@
       <c r="F2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -473,8 +482,11 @@
       <c r="F3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -493,8 +505,11 @@
       <c r="F4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -513,8 +528,11 @@
       <c r="F5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -533,8 +551,11 @@
       <c r="F6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -553,8 +574,11 @@
       <c r="F7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -573,8 +597,11 @@
       <c r="F8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -593,8 +620,11 @@
       <c r="F9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -613,8 +643,11 @@
       <c r="F10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -633,8 +666,11 @@
       <c r="F11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -653,8 +689,11 @@
       <c r="F12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -673,8 +712,11 @@
       <c r="F13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -693,8 +735,11 @@
       <c r="F14" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -713,8 +758,11 @@
       <c r="F15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -733,8 +781,11 @@
       <c r="F16" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -753,8 +804,11 @@
       <c r="F17" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <f>A17+1</f>
         <v>16</v>
@@ -774,8 +828,11 @@
       <c r="F18" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ref="A19:A42" si="0">A18+1</f>
         <v>17</v>
@@ -795,8 +852,11 @@
       <c r="F19" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -816,8 +876,11 @@
       <c r="F20" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -837,8 +900,11 @@
       <c r="F21" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -858,8 +924,11 @@
       <c r="F22" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -879,8 +948,11 @@
       <c r="F23" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -900,8 +972,11 @@
       <c r="F24" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -921,8 +996,11 @@
       <c r="F25" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -942,8 +1020,11 @@
       <c r="F26" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -963,8 +1044,11 @@
       <c r="F27" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -984,8 +1068,11 @@
       <c r="F28" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1005,8 +1092,11 @@
       <c r="F29" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1026,8 +1116,11 @@
       <c r="F30" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1047,8 +1140,11 @@
       <c r="F31" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1068,8 +1164,11 @@
       <c r="F32" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1089,8 +1188,11 @@
       <c r="F33" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1110,8 +1212,11 @@
       <c r="F34" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1131,8 +1236,11 @@
       <c r="F35" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1152,8 +1260,11 @@
       <c r="F36" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1173,8 +1284,11 @@
       <c r="F37" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1194,8 +1308,11 @@
       <c r="F38" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1215,8 +1332,11 @@
       <c r="F39" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1236,8 +1356,11 @@
       <c r="F40" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1257,8 +1380,11 @@
       <c r="F41" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1276,6 +1402,9 @@
         <v>0</v>
       </c>
       <c r="F42" t="s">
+        <v>6</v>
+      </c>
+      <c r="G42" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added final cards, implemented high score and tips
</commit_message>
<xml_diff>
--- a/Card_Data.xlsx
+++ b/Card_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samya\Documents\Programming\Github_Repos\Y3Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DFC2E88-CA7D-4C57-8587-8826BFFB5F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196210CA-895B-4287-8BE2-F375F70ECA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{19CA79AA-259F-45F1-9CD4-466022CA0906}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="9">
   <si>
     <t>ID</t>
   </si>
@@ -403,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DA40240-B6B9-4147-8877-CA9E78CDE18C}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,6 +1408,121 @@
         <v>6</v>
       </c>
     </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>10</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>15</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <v>-10</v>
+      </c>
+      <c r="D44">
+        <v>5</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>10</v>
+      </c>
+      <c r="C45">
+        <v>-10</v>
+      </c>
+      <c r="D45">
+        <v>10</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>-10</v>
+      </c>
+      <c r="C46">
+        <v>-10</v>
+      </c>
+      <c r="D46">
+        <v>10</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>-10</v>
+      </c>
+      <c r="C47">
+        <v>-5</v>
+      </c>
+      <c r="D47">
+        <v>10</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>6</v>
+      </c>
+      <c r="G47" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>